<commit_message>
Make Buffer Output for Summary Sheet
</commit_message>
<xml_diff>
--- a/PreventiveMaintenance.xlsx
+++ b/PreventiveMaintenance.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>Hostname</t>
   </si>
@@ -64,7 +64,7 @@
     <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
   </si>
   <si>
-    <t>4 weeks, 4 days, 3 hours, 52 minutes</t>
+    <t>4 weeks, 5 days, 3 hours, 39 minutes</t>
   </si>
   <si>
     <t>1648789K</t>
@@ -184,16 +184,13 @@
     <t>Excellent</t>
   </si>
   <si>
-    <t>5%/0%</t>
+    <t>2%/0%</t>
   </si>
   <si>
     <t>1%</t>
   </si>
   <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>2%/0%</t>
+    <t>3%/0%</t>
   </si>
   <si>
     <t>Variable</t>
@@ -1076,13 +1073,13 @@
         <v>1688360784</v>
       </c>
       <c r="C3" t="n">
-        <v>408167328</v>
+        <v>408167224</v>
       </c>
       <c r="D3" t="n">
-        <v>1280193456</v>
+        <v>1280193560</v>
       </c>
       <c r="E3" t="n">
-        <v>24.17536179873744</v>
+        <v>24.17535563891657</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -1094,7 +1091,7 @@
         <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J3" t="s">
         <v>54</v>
@@ -1108,25 +1105,25 @@
         <v>1688360784</v>
       </c>
       <c r="C4" t="n">
-        <v>405609952</v>
+        <v>405610100</v>
       </c>
       <c r="D4" t="n">
-        <v>1282750832</v>
+        <v>1282750684</v>
       </c>
       <c r="E4" t="n">
-        <v>24.02389085578287</v>
+        <v>24.02389962168181</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>54</v>
@@ -1162,19 +1159,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>49</v>
@@ -1185,16 +1182,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="n">
-        <v>11255223</v>
+        <v>11597010</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>11255223</v>
+        <v>11597010</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1205,16 +1202,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="n">
-        <v>11211933</v>
+        <v>11569317</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>11211933</v>
+        <v>11569317</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1225,19 +1222,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="n">
-        <v>2506484</v>
+        <v>2583853</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>2506490</v>
+        <v>2583859</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0002393785732239107</v>
+        <v>0.0002322108133609458</v>
       </c>
       <c r="G4" t="s">
         <v>54</v>
@@ -1245,19 +1242,19 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" t="n">
-        <v>1667202</v>
+        <v>1718549</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>1667210</v>
+        <v>1718557</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0004798435709958553</v>
+        <v>0.0004655068176382861</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
@@ -1265,7 +1262,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
@@ -1285,7 +1282,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -1308,16 +1305,16 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="n">
-        <v>11281571</v>
+        <v>11626592</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>11281571</v>
+        <v>11626592</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1328,16 +1325,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="n">
-        <v>11214586</v>
+        <v>11571534</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>11214586</v>
+        <v>11571534</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1348,19 +1345,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="n">
-        <v>2508094</v>
+        <v>2585247</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>2508096</v>
+        <v>2585249</v>
       </c>
       <c r="F10" t="n">
-        <v>7.974176427058614e-05</v>
+        <v>7.736198718189234e-05</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
@@ -1368,19 +1365,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="n">
-        <v>1667207</v>
+        <v>1718555</v>
       </c>
       <c r="D11" t="n">
         <v>8</v>
       </c>
       <c r="E11" t="n">
-        <v>1667215</v>
+        <v>1718563</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0004798421319385922</v>
+        <v>0.0004655051924194807</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
@@ -1388,7 +1385,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="n">
         <v>8</v>
@@ -1408,7 +1405,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -1456,10 +1453,10 @@
         <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1472,6 +1469,9 @@
       <c r="C2" t="s">
         <v>54</v>
       </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -1481,6 +1481,9 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make Output for Column Conclusion
</commit_message>
<xml_diff>
--- a/PreventiveMaintenance.xlsx
+++ b/PreventiveMaintenance.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>Hostname</t>
   </si>
@@ -64,7 +64,7 @@
     <t>X86_64_LINUX_IOSD-UNIVERSALK9-M</t>
   </si>
   <si>
-    <t>4 weeks, 5 days, 3 hours, 39 minutes</t>
+    <t>5 weeks, 20 hours, 2 minutes</t>
   </si>
   <si>
     <t>1648789K</t>
@@ -190,7 +190,7 @@
     <t>1%</t>
   </si>
   <si>
-    <t>3%/0%</t>
+    <t>0%/0%</t>
   </si>
   <si>
     <t>Variable</t>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Conclusion</t>
+  </si>
+  <si>
+    <t>No Action Required</t>
   </si>
 </sst>
 </file>
@@ -1073,13 +1076,13 @@
         <v>1688360784</v>
       </c>
       <c r="C3" t="n">
-        <v>408167224</v>
+        <v>408167092</v>
       </c>
       <c r="D3" t="n">
-        <v>1280193560</v>
+        <v>1280193692</v>
       </c>
       <c r="E3" t="n">
-        <v>24.17535563891657</v>
+        <v>24.17534782068238</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -1105,13 +1108,13 @@
         <v>1688360784</v>
       </c>
       <c r="C4" t="n">
-        <v>405610100</v>
+        <v>405609460</v>
       </c>
       <c r="D4" t="n">
-        <v>1282750684</v>
+        <v>1282751324</v>
       </c>
       <c r="E4" t="n">
-        <v>24.02389962168181</v>
+        <v>24.02386171509182</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -1185,13 +1188,13 @@
         <v>62</v>
       </c>
       <c r="C2" t="n">
-        <v>11597010</v>
+        <v>12498808</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>11597010</v>
+        <v>12498808</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1205,13 +1208,13 @@
         <v>63</v>
       </c>
       <c r="C3" t="n">
-        <v>11569317</v>
+        <v>12500046</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>11569317</v>
+        <v>12500046</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1225,16 +1228,16 @@
         <v>64</v>
       </c>
       <c r="C4" t="n">
-        <v>2583853</v>
+        <v>2792974</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>2583859</v>
+        <v>2792980</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0002322108133609458</v>
+        <v>0.0002148243095188651</v>
       </c>
       <c r="G4" t="s">
         <v>54</v>
@@ -1245,16 +1248,16 @@
         <v>65</v>
       </c>
       <c r="C5" t="n">
-        <v>1718549</v>
+        <v>1857594</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>1718557</v>
+        <v>1857602</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0004655068176382861</v>
+        <v>0.0004306627576843695</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
@@ -1308,13 +1311,13 @@
         <v>62</v>
       </c>
       <c r="C8" t="n">
-        <v>11626592</v>
+        <v>12531575</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>11626592</v>
+        <v>12531575</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1328,13 +1331,13 @@
         <v>63</v>
       </c>
       <c r="C9" t="n">
-        <v>11571534</v>
+        <v>12502447</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>11571534</v>
+        <v>12502447</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1348,16 +1351,16 @@
         <v>64</v>
       </c>
       <c r="C10" t="n">
-        <v>2585247</v>
+        <v>2793926</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>2585249</v>
+        <v>2793928</v>
       </c>
       <c r="F10" t="n">
-        <v>7.736198718189234e-05</v>
+        <v>7.158380602506579e-05</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
@@ -1368,16 +1371,16 @@
         <v>65</v>
       </c>
       <c r="C11" t="n">
-        <v>1718555</v>
+        <v>1857603</v>
       </c>
       <c r="D11" t="n">
         <v>8</v>
       </c>
       <c r="E11" t="n">
-        <v>1718563</v>
+        <v>1857611</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0004655051924194807</v>
+        <v>0.0004306606711523564</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
@@ -1472,6 +1475,9 @@
       <c r="D2" t="s">
         <v>54</v>
       </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -1485,6 +1491,9 @@
       </c>
       <c r="D3" t="s">
         <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>